<commit_message>
added type column; made 4 owned col not required
</commit_message>
<xml_diff>
--- a/tests/data/test_update_missing_metadata.xlsx
+++ b/tests/data/test_update_missing_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\local_documents\GitHub Projects\PokemonExcelParser\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D953D58-8583-44CA-B297-CFCEF02D1046}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EBD781-E70B-4E26-8CF7-3E28EA16AEA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{78BC78BC-29BB-4F6D-966B-C0ED778393B8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Card #</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Rarity</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -399,15 +402,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C793CC09-1384-4169-8F40-1E1A627FBB9C}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -420,8 +423,11 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1</v>
       </c>
@@ -429,7 +435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2</v>
       </c>
@@ -437,7 +443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>3</v>
       </c>
@@ -445,7 +451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
changed 4 Owned column to # owned
</commit_message>
<xml_diff>
--- a/tests/data/test_update_missing_metadata.xlsx
+++ b/tests/data/test_update_missing_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\local_documents\GitHub Projects\PokemonExcelParser\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EBD781-E70B-4E26-8CF7-3E28EA16AEA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797E6806-6720-43AD-84A3-BE6C5E53F812}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{78BC78BC-29BB-4F6D-966B-C0ED778393B8}"/>
   </bookViews>
@@ -33,15 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Card #</t>
-  </si>
-  <si>
-    <t>4 Owned</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>Name</t>
@@ -51,6 +45,9 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t># Owned</t>
   </si>
 </sst>
 </file>
@@ -405,58 +402,58 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
+      <c r="C2">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
+      <c r="C3">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>2</v>
+      <c r="C4">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>2</v>
+      <c r="C5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>